<commit_message>
Aug 04 2023 changes
</commit_message>
<xml_diff>
--- a/Training Calendar.xlsx
+++ b/Training Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajesh\Training\Aug 2023 Salesforce Admin &amp; Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA05580C-FEC7-4DBB-AB96-C5BA55704833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E1DB9D-CC6A-4410-A12E-1D3895EB34A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BD14083-DB89-4F23-8AD4-E7E30FE542D5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>Yet to start</t>
+  </si>
+  <si>
+    <t>https://meet.jit.si/DelightedMuseumsRuinThrough</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +164,21 @@
     <font>
       <sz val="9.6"/>
       <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,10 +242,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -238,13 +257,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -253,8 +269,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,7 +596,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,17 +605,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="25.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,257 +639,259 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5">
-        <v>3</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="5">
-        <v>3</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5">
-        <v>3</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5">
-        <v>3</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4">
         <v>0</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4">
         <v>0</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5">
-        <v>3</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5">
-        <v>3</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="5">
-        <v>3</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <f>SUM(D3:D15)</f>
         <v>30</v>
       </c>
@@ -872,6 +900,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{36B111A2-2F6C-4E9F-A1DF-CA2523EB7BE5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added notes and Hands on
</commit_message>
<xml_diff>
--- a/Training Calendar.xlsx
+++ b/Training Calendar.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajesh\Training\Aug 2023 Salesforce Admin &amp; Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajesh\Week End Training Session\Aug 2023 Salesforce Admin &amp; Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E1DB9D-CC6A-4410-A12E-1D3895EB34A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F09C23-5B06-4EB0-B419-C83DD07C8DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BD14083-DB89-4F23-8AD4-E7E30FE542D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
+    <sheet name="Curriculum" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -57,21 +58,12 @@
     <t>Aug 06, 2023</t>
   </si>
   <si>
-    <t>Aug 12, 2023</t>
-  </si>
-  <si>
-    <t>Aug 13, 2023</t>
-  </si>
-  <si>
     <t>Aug 19, 2023</t>
   </si>
   <si>
     <t>Aug 20, 2023</t>
   </si>
   <si>
-    <t>Aug 26, 2023</t>
-  </si>
-  <si>
     <t>Aug 27, 2023</t>
   </si>
   <si>
@@ -102,13 +94,43 @@
     <t>Not Available</t>
   </si>
   <si>
-    <t>In Progess</t>
-  </si>
-  <si>
     <t>Yet to start</t>
   </si>
   <si>
     <t>https://meet.jit.si/DelightedMuseumsRuinThrough</t>
+  </si>
+  <si>
+    <t>7:00 - 8:30 P.M</t>
+  </si>
+  <si>
+    <t>1.5 hours</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>https://meet.jit.si/LimitedAdsShiftAbsolutely</t>
+  </si>
+  <si>
+    <t>Aug 23, 2023</t>
+  </si>
+  <si>
+    <t>Aug 24, 2023</t>
+  </si>
+  <si>
+    <t>Sep 23, 2023</t>
+  </si>
+  <si>
+    <t>2:30 AM - 5:30 PM</t>
+  </si>
+  <si>
+    <t>Aug 30, 2023</t>
+  </si>
+  <si>
+    <t>Aug 31, 2023</t>
+  </si>
+  <si>
+    <t>Buffer</t>
   </si>
 </sst>
 </file>
@@ -246,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -269,15 +291,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,27 +622,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59B0CC0-C030-4F9C-A0E6-78573C425839}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="A1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -626,12 +656,12 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -651,11 +681,11 @@
       <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>27</v>
+      <c r="E3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -673,13 +703,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="F4" s="12"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -691,53 +721,59 @@
       <c r="D5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="4">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D7" s="4">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -748,15 +784,17 @@
       <c r="D8" s="4">
         <v>3</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -767,53 +805,59 @@
       <c r="D9" s="4">
         <v>3</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D10" s="4">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -825,17 +869,19 @@
         <v>0</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>8</v>
@@ -844,14 +890,16 @@
         <v>3</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
@@ -863,14 +911,16 @@
         <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
@@ -882,17 +932,61 @@
         <v>3</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="6">
-        <f>SUM(D3:D15)</f>
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="6">
+        <f>SUM(D3:D17)</f>
         <v>30</v>
       </c>
     </row>
@@ -902,7 +996,34 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{36B111A2-2F6C-4E9F-A1DF-CA2523EB7BE5}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{C873AA91-FC03-4E40-AB8F-40BC931F0EDE}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{38B439A1-9018-408A-8FE0-467E69B768FD}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{A67208DE-BA73-49CD-BE9D-152CE6C06748}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{F7EBB18D-2CB4-4295-A7DA-34BD724462E0}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{72939A6D-C42F-4ED9-934A-357E9F1BDEB9}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{95899F4C-F69C-4B94-9405-85A13199B17F}"/>
+    <hyperlink ref="F11" r:id="rId8" xr:uid="{4ADE42FB-4317-4D08-A58E-502F37A08BF2}"/>
+    <hyperlink ref="F12:F17" r:id="rId9" display="https://meet.jit.si/LimitedAdsShiftAbsolutely" xr:uid="{48E320C9-1542-4BBF-B34E-5F62DFBF47C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481E5B46-C3E9-4938-9D32-40104B3EBCFE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added sep 10 2023
</commit_message>
<xml_diff>
--- a/Training Calendar.xlsx
+++ b/Training Calendar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajesh\Week End Training Session\Aug 2023 Salesforce Admin &amp; Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F09C23-5B06-4EB0-B419-C83DD07C8DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AC36E8-648C-44F8-B75C-8D85833CD3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BD14083-DB89-4F23-8AD4-E7E30FE542D5}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>Aug 24, 2023</t>
   </si>
   <si>
-    <t>Sep 23, 2023</t>
-  </si>
-  <si>
     <t>2:30 AM - 5:30 PM</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Buffer</t>
+  </si>
+  <si>
+    <t>Sep 17, 2023</t>
   </si>
 </sst>
 </file>
@@ -268,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -297,16 +297,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -625,25 +624,25 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -661,7 +660,7 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -705,7 +704,7 @@
       <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -815,7 +814,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>24</v>
@@ -826,8 +825,8 @@
       <c r="D10" s="4">
         <v>1.5</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>22</v>
+      <c r="E10" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>27</v>
@@ -836,7 +835,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>24</v>
@@ -847,8 +846,8 @@
       <c r="D11" s="4">
         <v>1.5</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>22</v>
+      <c r="E11" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>27</v>
@@ -868,8 +867,8 @@
       <c r="D12" s="4">
         <v>0</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>21</v>
+      <c r="E12" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>27</v>
@@ -881,7 +880,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>8</v>
@@ -889,8 +888,8 @@
       <c r="D13" s="4">
         <v>3</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>22</v>
+      <c r="E13" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>27</v>
@@ -910,8 +909,8 @@
       <c r="D14" s="4">
         <v>3</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>22</v>
+      <c r="E14" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>27</v>
@@ -931,8 +930,8 @@
       <c r="D15" s="4">
         <v>3</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>22</v>
+      <c r="E15" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>27</v>
@@ -962,7 +961,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -974,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Added notes Sep 30 2023
</commit_message>
<xml_diff>
--- a/Training Calendar.xlsx
+++ b/Training Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajesh\Week End Training Session\Aug 2023 Salesforce Admin &amp; Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BA1FA8-1029-4624-B4A4-75560B14C306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFDBDED-2A6E-47D5-BA85-3FA75B36BBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BD14083-DB89-4F23-8AD4-E7E30FE542D5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>2.5 hours</t>
+  </si>
+  <si>
+    <t>Sep 30, 2024</t>
   </si>
 </sst>
 </file>
@@ -627,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59B0CC0-C030-4F9C-A0E6-78573C425839}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,16 +1000,39 @@
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C21" s="5" t="s">
+      <c r="F21" s="9"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" s="9"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="6">
-        <f>SUM(D3:D19)</f>
-        <v>38</v>
+      <c r="D23" s="6">
+        <f>SUM(D3:D20)</f>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Notes and uses cases
</commit_message>
<xml_diff>
--- a/Training Calendar.xlsx
+++ b/Training Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajesh\Week End Training Session\Aug 2023 Salesforce Admin &amp; Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9D1451-E59D-4B43-A979-EEF25E697CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FC29D5-C20D-4404-ABAF-A6CAEEF8380A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BD14083-DB89-4F23-8AD4-E7E30FE542D5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>2 hours</t>
+  </si>
+  <si>
+    <t>Oct 28, 2024</t>
   </si>
 </sst>
 </file>
@@ -654,7 +657,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,6 +1098,23 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C26" s="5" t="s">

</xml_diff>